<commit_message>
BigOp is PERFECT. Yay!
</commit_message>
<xml_diff>
--- a/SqlServerScripter/SqlServerScripter/TableList.xlsx
+++ b/SqlServerScripter/SqlServerScripter/TableList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="26">
   <si>
     <t>TableName</t>
   </si>
@@ -50,9 +50,6 @@
     <t>dbo</t>
   </si>
   <si>
-    <t>tblTimeHistDetail</t>
-  </si>
-  <si>
     <t>RecordID</t>
   </si>
   <si>
@@ -99,6 +96,12 @@
   </si>
   <si>
     <t>id1</t>
+  </si>
+  <si>
+    <t>tblTimeHistDetailOld</t>
+  </si>
+  <si>
+    <t>tblAdjustments</t>
   </si>
 </sst>
 </file>
@@ -114,12 +117,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -134,8 +143,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,17 +460,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="11.3828125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.69140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.15234375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.07421875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.4609375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.3828125" bestFit="1" customWidth="1"/>
@@ -468,7 +478,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
@@ -491,53 +501,53 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G3" t="s">
-        <v>10</v>
+      <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -546,21 +556,21 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -569,21 +579,21 @@
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -592,21 +602,21 @@
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -615,21 +625,21 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
         <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -638,21 +648,21 @@
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
       </c>
       <c r="F9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -661,21 +671,21 @@
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s">
         <v>15</v>
       </c>
       <c r="F10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -684,39 +694,16 @@
         <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E11" t="s">
         <v>16</v>
       </c>
       <c r="F11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
One minor fix done
</commit_message>
<xml_diff>
--- a/SqlServerScripter/SqlServerScripter/TableList.xlsx
+++ b/SqlServerScripter/SqlServerScripter/TableList.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25714" windowHeight="12291" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25714" windowHeight="12291" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="SampleTableList" sheetId="1" r:id="rId1"/>
     <sheet name="RealTableList-1" sheetId="2" r:id="rId2"/>
     <sheet name="RealTableList-TC" sheetId="3" r:id="rId3"/>
     <sheet name="RealTableList-TH" sheetId="4" r:id="rId4"/>
-    <sheet name="RealTableList" sheetId="5" r:id="rId5"/>
+    <sheet name="RealTableList-TH1" sheetId="5" r:id="rId5"/>
+    <sheet name="RealTableList" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'RealTableList-1'!$A$1:$G$198</definedName>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2975" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2989" uniqueCount="189">
   <si>
     <t>TableName</t>
   </si>
@@ -10477,7 +10478,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H32" sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
@@ -10861,4 +10864,72 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="11.3828125" customWidth="1"/>
+    <col min="3" max="3" width="11.69140625" customWidth="1"/>
+    <col min="4" max="4" width="18.765625" customWidth="1"/>
+    <col min="5" max="5" width="12.07421875" customWidth="1"/>
+    <col min="6" max="6" width="11.4609375" customWidth="1"/>
+    <col min="7" max="7" width="12.3828125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>